<commit_message>
Cleaner code generation, npytyping type hints for arrays
- split off generated subclasses into "include" files, not sure if that's good, but in any case we have them separable now.
- more work on cleanly un-nesting scalar and 1D-vector data into attributes and lists, respectively
- brought the pydantic generator in-repo to do a bunch of overrides
</commit_message>
<xml_diff>
--- a/nwb_schema_language/project/excel/nwb_schema_language.xlsx
+++ b/nwb_schema_language/project/excel/nwb_schema_language.xlsx
@@ -547,11 +547,6 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"float,float32,double,float64,long,int64,int,int32,int16,short,int8,uint,uint32,uint16,uint8,uint64,numeric,text,utf,utf8,utf-8,ascii,bool,isodatetime"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>